<commit_message>
Reorganized code. Ready to submit.
</commit_message>
<xml_diff>
--- a/MPI/performance/performance.xlsx
+++ b/MPI/performance/performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Gits Storage\UW\CSS534-Final-Project\MPI\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D300DC0-7198-4EDE-88C7-52FB1C3475F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AC4639-2C7C-455F-960B-1C79881FA9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7935" yWindow="1770" windowWidth="28800" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Node #</t>
   </si>
@@ -55,18 +55,6 @@
   <si>
     <t>Time KNN</t>
   </si>
-  <si>
-    <t>求和</t>
-  </si>
-  <si>
-    <t>平均值</t>
-  </si>
-  <si>
-    <t>汇总</t>
-  </si>
-  <si>
-    <t>计数</t>
-  </si>
 </sst>
 </file>
 
@@ -76,8 +64,16 @@
     <numFmt numFmtId="164" formatCode="yyyy/m/d\ h:mm;@"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,7 +89,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -101,15 +97,206 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -222,7 +409,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="bg1">
                   <a:lumMod val="50000"/>
@@ -233,8 +420,78 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$9</c:f>
@@ -323,19 +580,88 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="15875" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="star"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$9</c:f>
@@ -424,7 +750,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -448,6 +774,72 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.1507101316251622E-2"/>
+                  <c:y val="2.4296665398307521E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-B361-4C78-A9BF-32909806D782}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.6983667112769705E-2"/>
+                  <c:y val="2.1737106271282541E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-B361-4C78-A9BF-32909806D782}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.6276980980576952E-3"/>
+                  <c:y val="6.3797515091321847E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-B361-4C78-A9BF-32909806D782}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -593,20 +985,89 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="15875" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5">
                   <a:lumMod val="60000"/>
                   <a:lumOff val="40000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$9</c:f>
@@ -688,6 +1149,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1641991151"/>
         <c:axId val="1642002799"/>
@@ -1863,7 +2325,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1871,204 +2333,204 @@
     <col min="1" max="1" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="20" t="s">
         <v>4</v>
       </c>
       <c r="G1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="14">
         <v>38248</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="14">
         <v>2139</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="15">
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="14">
         <v>36109</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="16">
         <v>0</v>
       </c>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>36831</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>2861</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="5">
         <f>C3-C2</f>
         <v>722</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>16726</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="7">
         <v>17244</v>
       </c>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>24054</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>2998</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="5">
         <f>C4-C2</f>
         <v>859</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>9914</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="7">
         <v>11142</v>
       </c>
       <c r="G4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>18880</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>3259</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="5">
         <f>C5-C2</f>
         <v>1120</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>7176</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="7">
         <v>8445</v>
       </c>
       <c r="G5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>18414</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>3307</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="5">
         <f>C6-C2</f>
         <v>1168</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>5911</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="7">
         <v>9196</v>
       </c>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="5">
         <v>13981</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="5">
         <v>3208</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="5">
         <f>C7-C2</f>
         <v>1069</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="5">
         <v>4441</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="8">
         <v>6332</v>
       </c>
       <c r="G7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>12503</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>3218</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="5">
         <f>C8-C2</f>
         <v>1079</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <v>3792</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="7">
         <v>5493</v>
       </c>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="10">
         <v>12039</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="10">
         <v>3261</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="11">
         <f>C9-C2</f>
         <v>1122</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="10">
         <v>3251</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="12">
         <v>5524</v>
       </c>
       <c r="G9"/>

</xml_diff>